<commit_message>
update tooltip error message catch
</commit_message>
<xml_diff>
--- a/test-data/test_data.xlsx
+++ b/test-data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OussemaHADJABDALLAH\Downloads\ts-test-framework-latest-allure\ts-test-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1642DF2-2B96-4601-A366-1F6697034AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6945F5B3-3365-4F2E-BE8A-68F8D085E23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8928" xr2:uid="{68735DB2-467A-436E-ADFC-94D25B53B451}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>test_case_id</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>Valid Login</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-002</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-003</t>
+  </si>
+  <si>
+    <t>Invalid Username</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-004</t>
+  </si>
+  <si>
+    <t>Empty Credentials</t>
+  </si>
+  <si>
+    <t>testpwd</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -453,15 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFAC38A-31BE-41C7-ADE6-D829C518BA4F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
@@ -506,6 +534,60 @@
         <v>200</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>